<commit_message>
DESCW-1364 adds remaining templates
* should cover all models with a template now (excel)
* might be worth doing this with word
* ideally: do report in excel, then paste the table in word.
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/genericReportTemplate.xlsx
+++ b/backend/reports/xlsx/genericReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2652C26C-67AD-DE4B-9D81-82EBF2487CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F2D95-0CAF-9C4E-86F6-F58748A44EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -101,7 +101,7 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
@@ -208,7 +208,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -245,6 +244,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -311,7 +311,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:ext cx="2411614" cy="680356"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -626,7 +626,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+      <selection activeCell="B7" sqref="B7:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -637,91 +637,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="19">
+      <c r="B7" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:9" ht="19">
+      <c r="B8" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:9" ht="19">
+      <c r="B9" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
+    <row r="10" spans="1:9" ht="19">
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" ht="19">
+      <c r="B11" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:9" ht="19">
+      <c r="B12" s="16" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DESCW-1282 Contractor Utilization summary by resource type (Tab 5)
* https://apps.itsm.gov.bc.ca/jira/browse/DESCW-1282
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/genericReportTemplate.xlsx
+++ b/backend/reports/xlsx/genericReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F2D95-0CAF-9C4E-86F6-F58748A44EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE4D8BD-E17A-F245-A949-CA0C6474008A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,24 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
   </si>
   <si>
     <t>{#fy=d.fiscal_year}</t>
@@ -61,15 +46,21 @@
   <si>
     <t>Project ________ for {$fy} as of {$date}</t>
   </si>
+  <si>
+    <t>{#row=d.report[i]}</t>
+  </si>
+  <si>
+    <t>{#rows=d.report[i+1]}</t>
+  </si>
+  <si>
+    <t>{#totals=d.report_totals[i]}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,15 +75,6 @@
     <font>
       <b/>
       <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
@@ -126,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -144,19 +126,6 @@
       <top style="medium">
         <color rgb="FFBFBFBF"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color rgb="FFBFBFBF"/>
       </bottom>
@@ -185,66 +154,120 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FFBFBFBF"/>
       </right>
       <top style="medium">
-        <color rgb="FFBFBFBF"/>
+        <color rgb="FFA5A5A5"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -253,6 +276,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBFBFBF"/>
       <color rgb="FF003365"/>
       <color rgb="FFC5DAF1"/>
     </mruColors>
@@ -623,10 +647,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -636,99 +660,160 @@
     <col min="3" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
-        <v>7</v>
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="9" spans="1:16" ht="19">
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="19">
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="11" spans="1:16" ht="19">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="7" spans="1:9" ht="19">
-      <c r="B7" s="16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="19">
-      <c r="B8" s="16" t="s">
+    </row>
+    <row r="12" spans="1:16" ht="19">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" ht="19">
+      <c r="B13" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19">
-      <c r="B9" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="19">
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" ht="19">
-      <c r="B11" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="19">
-      <c r="B12" s="16" t="s">
-        <v>3</v>
+    <row r="14" spans="1:16" ht="19">
+      <c r="B14" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
descw-1282      update changelog & cleanup files
* delete scratch sql file
* update generic report template for clean & simple use
* clean up tab 5 report template formatting
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/genericReportTemplate.xlsx
+++ b/backend/reports/xlsx/genericReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE4D8BD-E17A-F245-A949-CA0C6474008A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D0F438-C3F8-D640-A2EE-2ED69A96E9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
-  </si>
-  <si>
     <t>{#row=d.report[i]}</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>{#totals=d.report_totals[i]}</t>
+  </si>
+  <si>
+    <t>________ for {$fy} as of {$date}</t>
   </si>
 </sst>
 </file>
@@ -73,18 +73,18 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
@@ -108,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -132,41 +132,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFBFBFBF"/>
       </left>
@@ -215,57 +180,32 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -650,170 +590,104 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="2"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="9" spans="1:16" ht="17">
+      <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-    </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="9" spans="1:16" ht="19">
-      <c r="B9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:16" ht="17">
+      <c r="B10" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="19">
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:16" ht="17">
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="19">
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="19">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" ht="19">
-      <c r="B13" s="5" t="s">
+    <row r="12" spans="1:16" ht="17">
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" ht="17">
+      <c r="B13" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="19">
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:16" ht="17">
+      <c r="B14" s="8" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>